<commit_message>
Testing LOL with a datasets of hard binary mnist.
</commit_message>
<xml_diff>
--- a/TempTest/results/Accuracy.xlsx
+++ b/TempTest/results/Accuracy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="52">
   <si>
     <t>MNIST Hard Binary Classification</t>
   </si>
@@ -119,9 +119,6 @@
     <t>AVERAGE</t>
   </si>
   <si>
-    <t>Last time</t>
-  </si>
-  <si>
     <t>TRIAL6</t>
   </si>
   <si>
@@ -170,16 +167,28 @@
     <t>TRIAL20</t>
   </si>
   <si>
-    <t>This time</t>
-  </si>
-  <si>
     <t>GMRALOL: LOL w/ fixed k = Kmax</t>
+  </si>
+  <si>
+    <t>This time (ntrials = 20)</t>
+  </si>
+  <si>
+    <t>Last time (ntrials = 5)</t>
+  </si>
+  <si>
+    <t>MNIST_HardBinary_T60K_t10K</t>
+  </si>
+  <si>
+    <t>pos-def err</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -327,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -341,6 +350,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AR39"/>
+  <dimension ref="B1:AS39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T5" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -633,19 +651,59 @@
     <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" customWidth="1"/>
+    <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:44">
+    <row r="1" spans="2:45">
+      <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:44">
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2">
+        <v>0.81710000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="2:45">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:45">
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:44">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>0.97019999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="2:45">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -676,8 +734,18 @@
       <c r="L5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:44">
+      <c r="S5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0.86270000000000002</v>
+      </c>
+      <c r="V5">
+        <v>0.86270000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:45">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -711,14 +779,15 @@
       <c r="L6">
         <v>0.98</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AO6" s="19" t="s">
         <v>48</v>
       </c>
+      <c r="AP6" s="19"/>
       <c r="AR6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:44">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:45">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -771,61 +840,61 @@
         <v>29</v>
       </c>
       <c r="Z7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA7" t="s">
         <v>32</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>33</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>34</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>35</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>36</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>37</v>
       </c>
-      <c r="AF7" t="s">
-        <v>38</v>
-      </c>
       <c r="AG7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH7" t="s">
         <v>40</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>41</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>42</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>43</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>44</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AM7" t="s">
         <v>45</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>46</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>47</v>
       </c>
       <c r="AO7" t="s">
         <v>30</v>
       </c>
       <c r="AP7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AR7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:44">
+    <row r="8" spans="2:45">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -848,7 +917,7 @@
         <v>8</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U8" s="5"/>
       <c r="V8" s="6"/>
@@ -870,12 +939,18 @@
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
       <c r="AN8" s="6"/>
-      <c r="AO8" s="5"/>
+      <c r="AO8" s="16" t="e">
+        <f>AVERAGE(U8:AN8)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="AP8" s="6"/>
       <c r="AQ8" s="6"/>
       <c r="AR8" s="7"/>
-    </row>
-    <row r="9" spans="2:44">
+      <c r="AS8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:45">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -911,12 +986,18 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AO9" s="8"/>
+      <c r="AO9" s="17" t="e">
+        <f>AVERAGE(U9:AN9)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="AP9" s="4"/>
       <c r="AQ9" s="4"/>
       <c r="AR9" s="9"/>
-    </row>
-    <row r="10" spans="2:44">
+      <c r="AS9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:45">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -932,11 +1013,21 @@
       <c r="T10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U10" s="8"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
+      <c r="U10" s="8">
+        <v>0.99519999999999997</v>
+      </c>
+      <c r="V10" s="4">
+        <v>0.996</v>
+      </c>
+      <c r="W10" s="4">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="X10" s="4">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>0.99760000000000004</v>
+      </c>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
@@ -952,12 +1043,20 @@
       <c r="AL10" s="4"/>
       <c r="AM10" s="4"/>
       <c r="AN10" s="4"/>
-      <c r="AO10" s="8"/>
+      <c r="AO10" s="17">
+        <f>AVERAGE(U10:AN10)</f>
+        <v>0.99712000000000012</v>
+      </c>
       <c r="AP10" s="4"/>
       <c r="AQ10" s="4"/>
-      <c r="AR10" s="9"/>
-    </row>
-    <row r="11" spans="2:44">
+      <c r="AR10">
+        <v>0.997</v>
+      </c>
+      <c r="AS10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:45">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -970,11 +1069,21 @@
       <c r="T11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="10"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
+      <c r="U11" s="10">
+        <v>0.98480000000000001</v>
+      </c>
+      <c r="V11" s="11">
+        <v>0.98480000000000001</v>
+      </c>
+      <c r="W11" s="11">
+        <v>0.98680000000000001</v>
+      </c>
+      <c r="X11" s="11">
+        <v>0.98760000000000003</v>
+      </c>
+      <c r="Y11" s="11">
+        <v>0.98960000000000004</v>
+      </c>
       <c r="Z11" s="11"/>
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
@@ -990,14 +1099,20 @@
       <c r="AL11" s="11"/>
       <c r="AM11" s="11"/>
       <c r="AN11" s="11"/>
-      <c r="AO11" s="10"/>
+      <c r="AO11" s="18">
+        <f>AVERAGE(U11:AN11)</f>
+        <v>0.98672000000000004</v>
+      </c>
       <c r="AP11" s="11"/>
       <c r="AQ11" s="11"/>
       <c r="AR11" s="12">
         <v>0.98740000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="2:44">
+      <c r="AS11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:45">
       <c r="B12" t="s">
         <v>19</v>
       </c>
@@ -1011,7 +1126,7 @@
         <v>9</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U12" s="5"/>
       <c r="V12" s="6"/>
@@ -1028,8 +1143,11 @@
       <c r="AP12" s="4"/>
       <c r="AQ12" s="4"/>
       <c r="AR12" s="9"/>
-    </row>
-    <row r="13" spans="2:44">
+      <c r="AS12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:45">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -1057,8 +1175,11 @@
       <c r="AP13" s="4"/>
       <c r="AQ13" s="4"/>
       <c r="AR13" s="9"/>
-    </row>
-    <row r="14" spans="2:44">
+      <c r="AS13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:45">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -1086,8 +1207,11 @@
       <c r="AP14" s="4"/>
       <c r="AQ14" s="4"/>
       <c r="AR14" s="9"/>
-    </row>
-    <row r="15" spans="2:44">
+      <c r="AS14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:45">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -1117,8 +1241,11 @@
       <c r="AR15" s="9">
         <v>0.96599999999999997</v>
       </c>
-    </row>
-    <row r="16" spans="2:44">
+      <c r="AS15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:45">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1129,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U16" s="8"/>
       <c r="V16" s="4"/>
@@ -1151,8 +1278,11 @@
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
       <c r="AR16" s="7"/>
-    </row>
-    <row r="17" spans="2:44">
+      <c r="AS16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:45">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1182,8 +1312,11 @@
       <c r="AP17" s="4"/>
       <c r="AQ17" s="4"/>
       <c r="AR17" s="9"/>
-    </row>
-    <row r="18" spans="2:44">
+      <c r="AS17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:45">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1213,8 +1346,11 @@
       <c r="AP18" s="4"/>
       <c r="AQ18" s="4"/>
       <c r="AR18" s="9"/>
-    </row>
-    <row r="19" spans="2:44">
+      <c r="AS18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:45">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -1246,8 +1382,11 @@
       <c r="AR19" s="9">
         <v>0.95569999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="2:44">
+      <c r="AS19" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:45">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -1258,7 +1397,7 @@
         <v>11</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U20" s="5">
         <v>0.99829999999999997</v>
@@ -1320,15 +1459,21 @@
       <c r="AN20" s="6">
         <v>0.99670000000000003</v>
       </c>
-      <c r="AO20" s="5">
+      <c r="AO20" s="16">
         <f>AVERAGE(U20:AN20)</f>
         <v>0.99799000000000004</v>
       </c>
-      <c r="AP20" s="6"/>
+      <c r="AP20" s="14">
+        <f>_xlfn.VAR.S(U20:AN20)</f>
+        <v>4.268315789473692E-6</v>
+      </c>
       <c r="AQ20" s="6"/>
       <c r="AR20" s="7"/>
-    </row>
-    <row r="21" spans="2:44">
+      <c r="AS20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:45">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -1398,15 +1543,21 @@
       <c r="AN21" s="4">
         <v>0.995</v>
       </c>
-      <c r="AO21" s="8">
+      <c r="AO21" s="17">
         <f>AVERAGE(U21:AN21)</f>
         <v>0.99683500000000014</v>
       </c>
-      <c r="AP21" s="4"/>
+      <c r="AP21" s="13">
+        <f t="shared" ref="AP21:AP23" si="0">_xlfn.VAR.S(U21:AN21)</f>
+        <v>2.8834473684210475E-6</v>
+      </c>
       <c r="AQ21" s="4"/>
       <c r="AR21" s="9"/>
-    </row>
-    <row r="22" spans="2:44">
+      <c r="AS21" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:45">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -1416,34 +1567,83 @@
       <c r="T22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U22" s="8"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
-      <c r="AD22" s="4"/>
-      <c r="AE22" s="4"/>
-      <c r="AF22" s="4"/>
-      <c r="AG22" s="4"/>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="4"/>
-      <c r="AJ22" s="4"/>
-      <c r="AK22" s="4"/>
-      <c r="AL22" s="4"/>
-      <c r="AM22" s="4"/>
-      <c r="AN22" s="4"/>
-      <c r="AO22" s="8"/>
-      <c r="AP22" s="4"/>
+      <c r="U22" s="8">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="V22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="W22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="X22" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="Z22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AA22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AB22" s="4">
+        <v>0.995</v>
+      </c>
+      <c r="AC22" s="4">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AE22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AG22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AH22" s="4">
+        <v>0.995</v>
+      </c>
+      <c r="AI22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AJ22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AK22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AL22" s="4">
+        <v>0.99829999999999997</v>
+      </c>
+      <c r="AM22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AN22" s="4">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="AO22" s="17">
+        <f>AVERAGE(U22:AN22)</f>
+        <v>0.99708500000000022</v>
+      </c>
+      <c r="AP22" s="13">
+        <f t="shared" si="0"/>
+        <v>3.115026315789414E-6</v>
+      </c>
       <c r="AQ22" s="4"/>
-      <c r="AR22">
+      <c r="AR22" s="9">
         <v>0.99570000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="2:44">
+      <c r="AS22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:45">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -1513,17 +1713,23 @@
       <c r="AN23" s="11">
         <v>0.94669999999999999</v>
       </c>
-      <c r="AO23" s="10">
+      <c r="AO23" s="18">
         <f>AVERAGE(U23:AN23)</f>
         <v>0.9237550000000001</v>
       </c>
-      <c r="AP23" s="11"/>
+      <c r="AP23" s="15">
+        <f t="shared" si="0"/>
+        <v>2.8724050000000008E-4</v>
+      </c>
       <c r="AQ23" s="11"/>
       <c r="AR23" s="12">
         <v>0.92369999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="2:44">
+      <c r="AS23" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:45">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -1534,7 +1740,7 @@
         <v>12</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U24" s="8"/>
       <c r="V24" s="4"/>
@@ -1545,8 +1751,11 @@
       <c r="AP24" s="4"/>
       <c r="AQ24" s="4"/>
       <c r="AR24" s="9"/>
-    </row>
-    <row r="25" spans="2:44">
+      <c r="AS24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:45">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -1565,8 +1774,11 @@
       <c r="AP25" s="4"/>
       <c r="AQ25" s="4"/>
       <c r="AR25" s="9"/>
-    </row>
-    <row r="26" spans="2:44">
+      <c r="AS25" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:45">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -1585,8 +1797,11 @@
       <c r="AP26" s="4"/>
       <c r="AQ26" s="4"/>
       <c r="AR26" s="9"/>
-    </row>
-    <row r="27" spans="2:44">
+      <c r="AS26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:45">
       <c r="S27" s="3" t="s">
         <v>12</v>
       </c>
@@ -1604,8 +1819,11 @@
       <c r="AR27" s="9">
         <v>0.85160000000000002</v>
       </c>
-    </row>
-    <row r="28" spans="2:44">
+      <c r="AS27" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:45">
       <c r="R28">
         <v>7</v>
       </c>
@@ -1613,7 +1831,7 @@
         <v>13</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U28" s="5"/>
       <c r="V28" s="6"/>
@@ -1639,8 +1857,11 @@
       <c r="AP28" s="6"/>
       <c r="AQ28" s="6"/>
       <c r="AR28" s="7"/>
-    </row>
-    <row r="29" spans="2:44">
+      <c r="AS28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:45">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -1674,8 +1895,11 @@
       <c r="AP29" s="4"/>
       <c r="AQ29" s="4"/>
       <c r="AR29" s="9"/>
-    </row>
-    <row r="30" spans="2:44">
+      <c r="AS29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:45">
       <c r="S30" s="2" t="s">
         <v>13</v>
       </c>
@@ -1706,8 +1930,11 @@
       <c r="AP30" s="4"/>
       <c r="AQ30" s="4"/>
       <c r="AR30" s="9"/>
-    </row>
-    <row r="31" spans="2:44">
+      <c r="AS30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:45">
       <c r="S31" s="3" t="s">
         <v>13</v>
       </c>
@@ -1740,8 +1967,11 @@
       <c r="AR31" s="12">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="32" spans="2:44">
+      <c r="AS31" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:45">
       <c r="R32">
         <v>8</v>
       </c>
@@ -1749,14 +1979,17 @@
         <v>14</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AO32" s="8"/>
       <c r="AP32" s="4"/>
       <c r="AQ32" s="4"/>
       <c r="AR32" s="9"/>
-    </row>
-    <row r="33" spans="18:44">
+      <c r="AS32" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="18:45">
       <c r="S33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1767,8 +2000,11 @@
       <c r="AP33" s="4"/>
       <c r="AQ33" s="4"/>
       <c r="AR33" s="9"/>
-    </row>
-    <row r="34" spans="18:44">
+      <c r="AS33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="18:45">
       <c r="S34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1779,8 +2015,11 @@
       <c r="AP34" s="4"/>
       <c r="AQ34" s="4"/>
       <c r="AR34" s="9"/>
-    </row>
-    <row r="35" spans="18:44">
+      <c r="AS34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="18:45">
       <c r="S35" s="3" t="s">
         <v>14</v>
       </c>
@@ -1793,8 +2032,11 @@
       <c r="AR35" s="9">
         <v>0.94930000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="18:44">
+      <c r="AS35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="18:45">
       <c r="R36">
         <v>9</v>
       </c>
@@ -1802,14 +2044,17 @@
         <v>15</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AO36" s="8"/>
       <c r="AP36" s="4"/>
       <c r="AQ36" s="4"/>
       <c r="AR36" s="9"/>
-    </row>
-    <row r="37" spans="18:44">
+      <c r="AS36" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="18:45">
       <c r="S37" s="2" t="s">
         <v>15</v>
       </c>
@@ -1820,8 +2065,11 @@
       <c r="AP37" s="4"/>
       <c r="AQ37" s="4"/>
       <c r="AR37" s="9"/>
-    </row>
-    <row r="38" spans="18:44">
+      <c r="AS37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="18:45">
       <c r="S38" s="2" t="s">
         <v>15</v>
       </c>
@@ -1832,8 +2080,11 @@
       <c r="AP38" s="4"/>
       <c r="AQ38" s="4"/>
       <c r="AR38" s="9"/>
-    </row>
-    <row r="39" spans="18:44">
+      <c r="AS38" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="18:45">
       <c r="S39" s="3" t="s">
         <v>15</v>
       </c>
@@ -1846,8 +2097,15 @@
       <c r="AR39" s="12">
         <v>0.98</v>
       </c>
+      <c r="AS39" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AO6:AP6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>